<commit_message>
clean manuscript with full render
</commit_message>
<xml_diff>
--- a/tables/supplementary_tables.xlsx
+++ b/tables/supplementary_tables.xlsx
@@ -270,6 +270,24 @@
     <t xml:space="preserve">rotting banana (on ground)</t>
   </si>
   <si>
+    <t xml:space="preserve">EG4724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agricultural_land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotting fruit, apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M. Ailion</t>
+  </si>
+  <si>
     <t xml:space="preserve">ECA248</t>
   </si>
   <si>
@@ -435,9 +453,6 @@
     <t xml:space="preserve">S-13424</t>
   </si>
   <si>
-    <t xml:space="preserve">Agricultural_land</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECA2656</t>
   </si>
   <si>
@@ -465,6 +480,12 @@
     <t xml:space="preserve">S-12494</t>
   </si>
   <si>
+    <t xml:space="preserve">EG4349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utah</t>
+  </si>
+  <si>
     <t xml:space="preserve">ECA36</t>
   </si>
   <si>
@@ -568,27 +589,6 @@
   </si>
   <si>
     <t xml:space="preserve">Isolated from compost from the Olive Mushroom Farms near the town of Limuru, Kenya;  altitude 2356m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EG4349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rotting fruit, apple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M. Ailion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EG4724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Braga</t>
   </si>
   <si>
     <t xml:space="preserve">JT11398</t>
@@ -5835,28 +5835,28 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C15" t="n">
         <v>20160408</v>
       </c>
       <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="n">
+        <v>41.6288</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-8.3476</v>
+      </c>
+      <c r="G15" t="s">
         <v>84</v>
       </c>
-      <c r="E15" t="n">
-        <v>37.44</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-122.14</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
         <v>86</v>
@@ -5871,36 +5871,36 @@
         <v>87</v>
       </c>
       <c r="P15" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>29952</v>
+        <v>39169</v>
       </c>
       <c r="R15" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
         <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>90</v>
       </c>
       <c r="C16" t="n">
         <v>20160408</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E16" t="n">
-        <v>34.096</v>
+        <v>37.44</v>
       </c>
       <c r="F16" t="n">
-        <v>-117.719</v>
+        <v>-122.14</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -5924,7 +5924,7 @@
         <v>19</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>26604</v>
+        <v>29952</v>
       </c>
       <c r="R16" t="s">
         <v>94</v>
@@ -5938,60 +5938,54 @@
         <v>96</v>
       </c>
       <c r="C17" t="n">
-        <v>20210121</v>
+        <v>20160408</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E17" t="n">
-        <v>-38.15055556</v>
+        <v>34.096</v>
       </c>
       <c r="F17" t="n">
-        <v>144.3788889</v>
+        <v>-117.719</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="L17" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="M17" t="n">
-        <v>69.7</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
       <c r="N17" t="s">
         <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="P17" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>43881</v>
+        <v>26604</v>
       </c>
       <c r="R17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" t="n">
         <v>20210121</v>
@@ -6000,10 +5994,10 @@
         <v>75</v>
       </c>
       <c r="E18" t="n">
-        <v>-37.8699364</v>
+        <v>-38.15055556</v>
       </c>
       <c r="F18" t="n">
-        <v>144.9838814</v>
+        <v>144.3788889</v>
       </c>
       <c r="G18" t="s">
         <v>50</v>
@@ -6018,36 +6012,36 @@
         <v>19</v>
       </c>
       <c r="K18" t="n">
-        <v>18</v>
+        <v>15.5</v>
       </c>
       <c r="L18" t="n">
-        <v>21.5</v>
+        <v>17.4</v>
       </c>
       <c r="M18" t="n">
-        <v>62.5</v>
+        <v>69.7</v>
       </c>
       <c r="N18" t="s">
         <v>19</v>
       </c>
       <c r="O18" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P18" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>43883</v>
+        <v>43881</v>
       </c>
       <c r="R18" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C19" t="n">
         <v>20210121</v>
@@ -6086,24 +6080,24 @@
         <v>19</v>
       </c>
       <c r="O19" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P19" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q19" s="2" t="n">
         <v>43883</v>
       </c>
       <c r="R19" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C20" t="n">
         <v>20210121</v>
@@ -6112,10 +6106,10 @@
         <v>75</v>
       </c>
       <c r="E20" t="n">
-        <v>-37.8700328</v>
+        <v>-37.8699364</v>
       </c>
       <c r="F20" t="n">
-        <v>144.983856</v>
+        <v>144.9838814</v>
       </c>
       <c r="G20" t="s">
         <v>50</v>
@@ -6133,33 +6127,33 @@
         <v>18</v>
       </c>
       <c r="L20" t="n">
-        <v>22.2</v>
+        <v>21.5</v>
       </c>
       <c r="M20" t="n">
-        <v>59.5</v>
+        <v>62.5</v>
       </c>
       <c r="N20" t="s">
         <v>19</v>
       </c>
       <c r="O20" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P20" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q20" s="2" t="n">
         <v>43883</v>
       </c>
       <c r="R20" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C21" t="n">
         <v>20210121</v>
@@ -6198,24 +6192,24 @@
         <v>19</v>
       </c>
       <c r="O21" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q21" s="2" t="n">
         <v>43883</v>
       </c>
       <c r="R21" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C22" t="n">
         <v>20210121</v>
@@ -6224,10 +6218,10 @@
         <v>75</v>
       </c>
       <c r="E22" t="n">
-        <v>-37.87</v>
+        <v>-37.8700328</v>
       </c>
       <c r="F22" t="n">
-        <v>144.9836111</v>
+        <v>144.983856</v>
       </c>
       <c r="G22" t="s">
         <v>50</v>
@@ -6242,36 +6236,36 @@
         <v>19</v>
       </c>
       <c r="K22" t="n">
-        <v>17.8</v>
+        <v>18</v>
       </c>
       <c r="L22" t="n">
         <v>22.2</v>
       </c>
       <c r="M22" t="n">
-        <v>60.9</v>
+        <v>59.5</v>
       </c>
       <c r="N22" t="s">
         <v>19</v>
       </c>
       <c r="O22" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P22" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q22" s="2" t="n">
         <v>43883</v>
       </c>
       <c r="R22" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C23" t="n">
         <v>20210121</v>
@@ -6280,10 +6274,10 @@
         <v>75</v>
       </c>
       <c r="E23" t="n">
-        <v>-37.8269983</v>
+        <v>-37.87</v>
       </c>
       <c r="F23" t="n">
-        <v>144.9798563</v>
+        <v>144.9836111</v>
       </c>
       <c r="G23" t="s">
         <v>50</v>
@@ -6292,42 +6286,42 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
       </c>
       <c r="K23" t="n">
-        <v>22.3</v>
+        <v>17.8</v>
       </c>
       <c r="L23" t="n">
-        <v>26.2</v>
+        <v>22.2</v>
       </c>
       <c r="M23" t="n">
-        <v>58.5</v>
+        <v>60.9</v>
       </c>
       <c r="N23" t="s">
         <v>19</v>
       </c>
       <c r="O23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="P23" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q23" s="2" t="n">
-        <v>43877</v>
+        <v>43883</v>
       </c>
       <c r="R23" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C24" t="n">
         <v>20210121</v>
@@ -6336,10 +6330,10 @@
         <v>75</v>
       </c>
       <c r="E24" t="n">
-        <v>-38.15</v>
+        <v>-37.8269983</v>
       </c>
       <c r="F24" t="n">
-        <v>144.3788889</v>
+        <v>144.9798563</v>
       </c>
       <c r="G24" t="s">
         <v>50</v>
@@ -6348,80 +6342,90 @@
         <v>19</v>
       </c>
       <c r="I24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J24" t="s">
         <v>19</v>
       </c>
       <c r="K24" t="n">
-        <v>18.7</v>
+        <v>22.3</v>
       </c>
       <c r="L24" t="n">
-        <v>18.8</v>
+        <v>26.2</v>
       </c>
       <c r="M24" t="n">
-        <v>67.6</v>
+        <v>58.5</v>
       </c>
       <c r="N24" t="s">
         <v>19</v>
       </c>
       <c r="O24" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="P24" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="Q24" s="2" t="n">
-        <v>43881</v>
+        <v>43877</v>
       </c>
       <c r="R24" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="n">
+        <v>20210121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-38.15</v>
+      </c>
+      <c r="F25" t="n">
+        <v>144.3788889</v>
+      </c>
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
         <v>118</v>
       </c>
-      <c r="C25" t="n">
-        <v>20160408</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" t="s">
-        <v>119</v>
-      </c>
       <c r="J25" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
+        <v>19</v>
+      </c>
+      <c r="K25" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="L25" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="M25" t="n">
+        <v>67.6</v>
+      </c>
       <c r="N25" t="s">
         <v>19</v>
       </c>
       <c r="O25" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="P25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q25" s="2" t="n">
-        <v>36127</v>
+        <v>43881</v>
       </c>
       <c r="R25" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26">
@@ -6432,60 +6436,50 @@
         <v>124</v>
       </c>
       <c r="C26" t="n">
-        <v>20210121</v>
+        <v>20160408</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" t="n">
-        <v>-37.83277778</v>
-      </c>
-      <c r="F26" t="n">
-        <v>144.9797222</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
         <v>19</v>
       </c>
       <c r="I26" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" t="n">
-        <v>22.1</v>
-      </c>
-      <c r="L26" t="n">
-        <v>27.6</v>
-      </c>
-      <c r="M26" t="n">
-        <v>54.1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
       <c r="N26" t="s">
         <v>19</v>
       </c>
       <c r="O26" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="P26" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="Q26" s="2" t="n">
-        <v>43877</v>
+        <v>36127</v>
       </c>
       <c r="R26" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C27" t="n">
         <v>20210121</v>
@@ -6494,10 +6488,10 @@
         <v>75</v>
       </c>
       <c r="E27" t="n">
-        <v>-37.8223566</v>
+        <v>-37.83277778</v>
       </c>
       <c r="F27" t="n">
-        <v>144.9736758</v>
+        <v>144.9797222</v>
       </c>
       <c r="G27" t="s">
         <v>50</v>
@@ -6506,42 +6500,42 @@
         <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="J27" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="K27" t="n">
-        <v>21.5</v>
+        <v>22.1</v>
       </c>
       <c r="L27" t="n">
-        <v>25.6</v>
+        <v>27.6</v>
       </c>
       <c r="M27" t="n">
-        <v>59.1</v>
+        <v>54.1</v>
       </c>
       <c r="N27" t="s">
         <v>19</v>
       </c>
       <c r="O27" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="P27" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="Q27" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R27" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C28" t="n">
         <v>20210121</v>
@@ -6550,10 +6544,10 @@
         <v>75</v>
       </c>
       <c r="E28" t="n">
-        <v>-37.82222222</v>
+        <v>-37.8223566</v>
       </c>
       <c r="F28" t="n">
-        <v>144.9736111</v>
+        <v>144.9736758</v>
       </c>
       <c r="G28" t="s">
         <v>50</v>
@@ -6562,42 +6556,42 @@
         <v>19</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="K28" t="n">
-        <v>22.2</v>
+        <v>21.5</v>
       </c>
       <c r="L28" t="n">
-        <v>26.2</v>
+        <v>25.6</v>
       </c>
       <c r="M28" t="n">
-        <v>56.9</v>
+        <v>59.1</v>
       </c>
       <c r="N28" t="s">
         <v>19</v>
       </c>
       <c r="O28" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="P28" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="Q28" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R28" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C29" t="n">
         <v>20210121</v>
@@ -6636,24 +6630,24 @@
         <v>19</v>
       </c>
       <c r="O29" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="P29" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q29" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R29" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C30" t="n">
         <v>20210121</v>
@@ -6662,10 +6656,10 @@
         <v>75</v>
       </c>
       <c r="E30" t="n">
-        <v>-37.825658</v>
+        <v>-37.82222222</v>
       </c>
       <c r="F30" t="n">
-        <v>144.9770918</v>
+        <v>144.9736111</v>
       </c>
       <c r="G30" t="s">
         <v>50</v>
@@ -6674,42 +6668,42 @@
         <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="J30" t="s">
         <v>19</v>
       </c>
       <c r="K30" t="n">
-        <v>23.3</v>
+        <v>22.2</v>
       </c>
       <c r="L30" t="n">
         <v>26.2</v>
       </c>
       <c r="M30" t="n">
-        <v>59.3</v>
+        <v>56.9</v>
       </c>
       <c r="N30" t="s">
         <v>19</v>
       </c>
       <c r="O30" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="P30" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="Q30" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R30" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C31" t="n">
         <v>20210121</v>
@@ -6718,19 +6712,19 @@
         <v>75</v>
       </c>
       <c r="E31" t="n">
-        <v>-37.82444444</v>
+        <v>-37.825658</v>
       </c>
       <c r="F31" t="n">
-        <v>145.4433333</v>
+        <v>144.9770918</v>
       </c>
       <c r="G31" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="H31" t="s">
         <v>19</v>
       </c>
       <c r="I31" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="J31" t="s">
         <v>19</v>
@@ -6739,33 +6733,33 @@
         <v>23.3</v>
       </c>
       <c r="L31" t="n">
-        <v>24.3</v>
+        <v>26.2</v>
       </c>
       <c r="M31" t="n">
-        <v>55.9</v>
+        <v>59.3</v>
       </c>
       <c r="N31" t="s">
         <v>19</v>
       </c>
       <c r="O31" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="P31" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="Q31" s="2" t="n">
-        <v>43882</v>
+        <v>43877</v>
       </c>
       <c r="R31" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C32" t="n">
         <v>20210121</v>
@@ -6774,19 +6768,19 @@
         <v>75</v>
       </c>
       <c r="E32" t="n">
-        <v>-37.825658</v>
+        <v>-37.82444444</v>
       </c>
       <c r="F32" t="n">
-        <v>144.9770918</v>
+        <v>145.4433333</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="J32" t="s">
         <v>19</v>
@@ -6795,33 +6789,33 @@
         <v>23.3</v>
       </c>
       <c r="L32" t="n">
-        <v>26.2</v>
+        <v>24.3</v>
       </c>
       <c r="M32" t="n">
-        <v>59.3</v>
+        <v>55.9</v>
       </c>
       <c r="N32" t="s">
         <v>19</v>
       </c>
       <c r="O32" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="P32" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="Q32" s="2" t="n">
-        <v>43877</v>
+        <v>43882</v>
       </c>
       <c r="R32" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C33" t="n">
         <v>20210121</v>
@@ -6830,10 +6824,10 @@
         <v>75</v>
       </c>
       <c r="E33" t="n">
-        <v>-37.8274278</v>
+        <v>-37.825658</v>
       </c>
       <c r="F33" t="n">
-        <v>144.980163</v>
+        <v>144.9770918</v>
       </c>
       <c r="G33" t="s">
         <v>50</v>
@@ -6842,42 +6836,42 @@
         <v>19</v>
       </c>
       <c r="I33" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="J33" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="K33" t="n">
-        <v>21.4</v>
+        <v>23.3</v>
       </c>
       <c r="L33" t="n">
         <v>26.2</v>
       </c>
       <c r="M33" t="n">
-        <v>58.9</v>
+        <v>59.3</v>
       </c>
       <c r="N33" t="s">
         <v>19</v>
       </c>
       <c r="O33" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P33" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="Q33" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R33" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C34" t="n">
         <v>20210121</v>
@@ -6901,7 +6895,7 @@
         <v>43</v>
       </c>
       <c r="J34" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="K34" t="n">
         <v>21.4</v>
@@ -6916,24 +6910,24 @@
         <v>19</v>
       </c>
       <c r="O34" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P34" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="Q34" s="2" t="n">
         <v>43877</v>
       </c>
       <c r="R34" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C35" t="n">
         <v>20210121</v>
@@ -6942,10 +6936,10 @@
         <v>75</v>
       </c>
       <c r="E35" t="n">
-        <v>-37.8701549</v>
+        <v>-37.8274278</v>
       </c>
       <c r="F35" t="n">
-        <v>144.9824148</v>
+        <v>144.980163</v>
       </c>
       <c r="G35" t="s">
         <v>50</v>
@@ -6957,113 +6951,119 @@
         <v>43</v>
       </c>
       <c r="J35" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="K35" t="n">
-        <v>19</v>
+        <v>21.4</v>
       </c>
       <c r="L35" t="n">
-        <v>20.8</v>
+        <v>26.2</v>
       </c>
       <c r="M35" t="n">
-        <v>64.4</v>
+        <v>58.9</v>
       </c>
       <c r="N35" t="s">
         <v>19</v>
       </c>
       <c r="O35" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="P35" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="Q35" s="2" t="n">
-        <v>43883</v>
+        <v>43877</v>
       </c>
       <c r="R35" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C36" t="n">
-        <v>20160408</v>
+        <v>20210121</v>
       </c>
       <c r="D36" t="s">
         <v>75</v>
       </c>
       <c r="E36" t="n">
-        <v>-36.893333</v>
+        <v>-37.8701549</v>
       </c>
       <c r="F36" t="n">
-        <v>174.745529</v>
+        <v>144.9824148</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H36" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J36" t="s">
-        <v>150</v>
-      </c>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
+        <v>19</v>
+      </c>
+      <c r="K36" t="n">
+        <v>19</v>
+      </c>
+      <c r="L36" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="M36" t="n">
+        <v>64.4</v>
+      </c>
       <c r="N36" t="s">
         <v>19</v>
       </c>
       <c r="O36" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="P36" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="Q36" s="2" t="n">
-        <v>41482</v>
+        <v>43883</v>
       </c>
       <c r="R36" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
       </c>
       <c r="C37" t="n">
-        <v>20170531</v>
+        <v>20160408</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E37" t="n">
-        <v>19.449831</v>
+        <v>40.771467</v>
       </c>
       <c r="F37" t="n">
-        <v>-155.235493</v>
+        <v>-111.87316</v>
       </c>
       <c r="G37" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="H37" t="s">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="I37" t="s">
         <v>43</v>
       </c>
       <c r="J37" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="K37"/>
       <c r="L37"/>
@@ -7072,13 +7072,13 @@
         <v>19</v>
       </c>
       <c r="O37" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
       <c r="P37" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="Q37" s="2" t="n">
-        <v>42507</v>
+        <v>38992</v>
       </c>
       <c r="R37" t="s">
         <v>19</v>
@@ -7086,34 +7086,34 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="C38" t="n">
-        <v>20180413</v>
+        <v>20160408</v>
       </c>
       <c r="D38" t="s">
         <v>75</v>
       </c>
       <c r="E38" t="n">
-        <v>34.417532</v>
+        <v>-36.893333</v>
       </c>
       <c r="F38" t="n">
-        <v>-119.640673</v>
+        <v>174.745529</v>
       </c>
       <c r="G38" t="s">
         <v>33</v>
       </c>
       <c r="H38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I38" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="J38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K38"/>
       <c r="L38"/>
@@ -7122,48 +7122,48 @@
         <v>19</v>
       </c>
       <c r="O38" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="P38" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="Q38" s="2" t="n">
-        <v>42801</v>
+        <v>41482</v>
       </c>
       <c r="R38" t="s">
-        <v>19</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="n">
-        <v>20180413</v>
+        <v>20170531</v>
       </c>
       <c r="D39" t="s">
         <v>75</v>
       </c>
       <c r="E39" t="n">
-        <v>34.065378</v>
+        <v>19.449831</v>
       </c>
       <c r="F39" t="n">
-        <v>-118.441156</v>
+        <v>-155.235493</v>
       </c>
       <c r="G39" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>161</v>
+        <v>42</v>
       </c>
       <c r="I39" t="s">
         <v>43</v>
       </c>
       <c r="J39" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K39"/>
       <c r="L39"/>
@@ -7172,13 +7172,13 @@
         <v>19</v>
       </c>
       <c r="O39" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="P39" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="Q39" s="2" t="n">
-        <v>42908</v>
+        <v>42507</v>
       </c>
       <c r="R39" t="s">
         <v>19</v>
@@ -7186,7 +7186,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -7198,22 +7198,22 @@
         <v>75</v>
       </c>
       <c r="E40" t="n">
-        <v>21.290067</v>
+        <v>34.417532</v>
       </c>
       <c r="F40" t="n">
-        <v>-157.707918</v>
+        <v>-119.640673</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
       </c>
       <c r="H40" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I40" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="J40" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K40"/>
       <c r="L40"/>
@@ -7222,13 +7222,13 @@
         <v>19</v>
       </c>
       <c r="O40" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="P40" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="Q40" s="2" t="n">
-        <v>43070</v>
+        <v>42801</v>
       </c>
       <c r="R40" t="s">
         <v>19</v>
@@ -7236,22 +7236,22 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>20160408</v>
+        <v>20180413</v>
       </c>
       <c r="D41" t="s">
-        <v>167</v>
+        <v>75</v>
       </c>
       <c r="E41" t="n">
-        <v>55.92</v>
+        <v>34.065378</v>
       </c>
       <c r="F41" t="n">
-        <v>-3.19</v>
+        <v>-118.441156</v>
       </c>
       <c r="G41" t="s">
         <v>33</v>
@@ -7260,10 +7260,10 @@
         <v>168</v>
       </c>
       <c r="I41" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="J41" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
@@ -7272,48 +7272,48 @@
         <v>19</v>
       </c>
       <c r="O41" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
       <c r="P41" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="Q41" s="2" t="n">
-        <v>38324</v>
+        <v>42908</v>
       </c>
       <c r="R41" t="s">
-        <v>171</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
       </c>
       <c r="C42" t="n">
-        <v>20160408</v>
+        <v>20180413</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>75</v>
       </c>
       <c r="E42" t="n">
-        <v>-33.366667</v>
+        <v>21.290067</v>
       </c>
       <c r="F42" t="n">
-        <v>19.316667</v>
+        <v>-157.707918</v>
       </c>
       <c r="G42" t="s">
         <v>33</v>
       </c>
       <c r="H42" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I42" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="J42" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
@@ -7322,21 +7322,21 @@
         <v>19</v>
       </c>
       <c r="O42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="P42" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="Q42" s="2" t="n">
-        <v>38842</v>
+        <v>43070</v>
       </c>
       <c r="R42" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -7345,25 +7345,25 @@
         <v>20160408</v>
       </c>
       <c r="D43" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E43" t="n">
-        <v>-33.366667</v>
+        <v>55.92</v>
       </c>
       <c r="F43" t="n">
-        <v>19.316667</v>
+        <v>-3.19</v>
       </c>
       <c r="G43" t="s">
         <v>33</v>
       </c>
       <c r="H43" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I43" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J43" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="K43"/>
       <c r="L43"/>
@@ -7372,21 +7372,21 @@
         <v>19</v>
       </c>
       <c r="O43" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P43" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="Q43" s="2" t="n">
-        <v>38809</v>
+        <v>38324</v>
       </c>
       <c r="R43" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
@@ -7395,7 +7395,7 @@
         <v>20160408</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E44" t="n">
         <v>-33.366667</v>
@@ -7407,13 +7407,13 @@
         <v>33</v>
       </c>
       <c r="H44" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="I44" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J44" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K44"/>
       <c r="L44"/>
@@ -7422,21 +7422,21 @@
         <v>19</v>
       </c>
       <c r="O44" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="P44" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="Q44" s="2" t="n">
-        <v>38809</v>
+        <v>38842</v>
       </c>
       <c r="R44" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -7445,7 +7445,7 @@
         <v>20160408</v>
       </c>
       <c r="D45" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E45" t="n">
         <v>-33.366667</v>
@@ -7457,13 +7457,13 @@
         <v>33</v>
       </c>
       <c r="H45" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="I45" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J45" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K45"/>
       <c r="L45"/>
@@ -7472,21 +7472,21 @@
         <v>19</v>
       </c>
       <c r="O45" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="P45" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="Q45" s="2" t="n">
-        <v>38842</v>
+        <v>38809</v>
       </c>
       <c r="R45" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -7495,25 +7495,25 @@
         <v>20160408</v>
       </c>
       <c r="D46" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E46" t="n">
-        <v>-1.083333</v>
+        <v>-33.366667</v>
       </c>
       <c r="F46" t="n">
-        <v>36.65</v>
+        <v>19.316667</v>
       </c>
       <c r="G46" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="H46" t="s">
         <v>180</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J46" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K46"/>
       <c r="L46"/>
@@ -7522,21 +7522,21 @@
         <v>19</v>
       </c>
       <c r="O46" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="P46" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="Q46" s="2" t="n">
-        <v>38854</v>
+        <v>38809</v>
       </c>
       <c r="R46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -7545,25 +7545,25 @@
         <v>20160408</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E47" t="n">
-        <v>40.771467</v>
+        <v>-33.366667</v>
       </c>
       <c r="F47" t="n">
-        <v>-111.87316</v>
+        <v>19.316667</v>
       </c>
       <c r="G47" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="H47" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I47" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="J47" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
       <c r="K47"/>
       <c r="L47"/>
@@ -7572,21 +7572,21 @@
         <v>19</v>
       </c>
       <c r="O47" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P47" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="Q47" s="2" t="n">
-        <v>38992</v>
+        <v>38842</v>
       </c>
       <c r="R47" t="s">
-        <v>19</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -7595,25 +7595,25 @@
         <v>20160408</v>
       </c>
       <c r="D48" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E48" t="n">
-        <v>41.6288</v>
+        <v>-1.083333</v>
       </c>
       <c r="F48" t="n">
-        <v>-8.3476</v>
+        <v>36.65</v>
       </c>
       <c r="G48" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I48" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="J48" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
       <c r="K48"/>
       <c r="L48"/>
@@ -7622,16 +7622,16 @@
         <v>19</v>
       </c>
       <c r="O48" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P48" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="Q48" s="2" t="n">
-        <v>39169</v>
+        <v>38854</v>
       </c>
       <c r="R48" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49">
@@ -7660,7 +7660,7 @@
         <v>191</v>
       </c>
       <c r="I49" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J49" t="s">
         <v>192</v>
@@ -7710,10 +7710,10 @@
         <v>198</v>
       </c>
       <c r="I50" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J50" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K50"/>
       <c r="L50"/>
@@ -7757,13 +7757,13 @@
         <v>41</v>
       </c>
       <c r="H51" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="I51" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J51" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K51"/>
       <c r="L51"/>
@@ -7810,7 +7810,7 @@
         <v>207</v>
       </c>
       <c r="I52" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J52" t="s">
         <v>208</v>
@@ -7863,7 +7863,7 @@
         <v>43</v>
       </c>
       <c r="J53" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K53"/>
       <c r="L53"/>
@@ -7954,16 +7954,16 @@
         <v>0.04619</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H55" t="s">
         <v>219</v>
       </c>
       <c r="I55" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J55" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K55"/>
       <c r="L55"/>
@@ -8113,7 +8113,7 @@
         <v>43</v>
       </c>
       <c r="J58" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K58"/>
       <c r="L58"/>
@@ -8163,7 +8163,7 @@
         <v>43</v>
       </c>
       <c r="J59" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K59"/>
       <c r="L59"/>
@@ -8460,10 +8460,10 @@
         <v>257</v>
       </c>
       <c r="I65" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J65" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K65"/>
       <c r="L65"/>
@@ -8554,7 +8554,7 @@
         <v>1.0512</v>
       </c>
       <c r="G67" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H67" t="s">
         <v>247</v>
@@ -8610,7 +8610,7 @@
         <v>247</v>
       </c>
       <c r="I68" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J68" t="s">
         <v>267</v>
@@ -8904,7 +8904,7 @@
         <v>-0.2685</v>
       </c>
       <c r="G74" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H74" t="s">
         <v>289</v>
@@ -9060,7 +9060,7 @@
         <v>215</v>
       </c>
       <c r="I77" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J77" t="s">
         <v>306</v>
@@ -9104,7 +9104,7 @@
         <v>-16.89</v>
       </c>
       <c r="G78" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H78" t="s">
         <v>309</v>
@@ -9160,7 +9160,7 @@
         <v>312</v>
       </c>
       <c r="I79" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J79" t="s">
         <v>313</v>
@@ -9254,7 +9254,7 @@
         <v>1.7915</v>
       </c>
       <c r="G81" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H81" t="s">
         <v>215</v>
@@ -9263,7 +9263,7 @@
         <v>43</v>
       </c>
       <c r="J81" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K81"/>
       <c r="L81"/>
@@ -9610,10 +9610,10 @@
         <v>228</v>
       </c>
       <c r="I88" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J88" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K88"/>
       <c r="L88"/>
@@ -9763,7 +9763,7 @@
         <v>43</v>
       </c>
       <c r="J91" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K91"/>
       <c r="L91"/>
@@ -9813,7 +9813,7 @@
         <v>43</v>
       </c>
       <c r="J92" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K92"/>
       <c r="L92"/>
@@ -9863,7 +9863,7 @@
         <v>43</v>
       </c>
       <c r="J93" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K93"/>
       <c r="L93"/>
@@ -9913,7 +9913,7 @@
         <v>43</v>
       </c>
       <c r="J94" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="K94"/>
       <c r="L94"/>
@@ -10260,7 +10260,7 @@
         <v>390</v>
       </c>
       <c r="I101" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J101" t="s">
         <v>391</v>
@@ -10360,7 +10360,7 @@
         <v>400</v>
       </c>
       <c r="I103" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J103" t="s">
         <v>401</v>
@@ -10410,10 +10410,10 @@
         <v>215</v>
       </c>
       <c r="I104" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J104" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K104"/>
       <c r="L104"/>
@@ -10504,7 +10504,7 @@
         <v>108.406</v>
       </c>
       <c r="G106" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H106" t="s">
         <v>411</v>
@@ -10560,7 +10560,7 @@
         <v>285</v>
       </c>
       <c r="I107" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J107" t="s">
         <v>414</v>
@@ -10710,7 +10710,7 @@
         <v>424</v>
       </c>
       <c r="I110" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J110" t="s">
         <v>425</v>
@@ -10860,10 +10860,10 @@
         <v>436</v>
       </c>
       <c r="I113" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J113" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K113"/>
       <c r="L113"/>
@@ -10910,10 +10910,10 @@
         <v>439</v>
       </c>
       <c r="I114" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J114" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K114"/>
       <c r="L114"/>
@@ -10960,10 +10960,10 @@
         <v>439</v>
       </c>
       <c r="I115" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J115" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K115"/>
       <c r="L115"/>
@@ -11010,10 +11010,10 @@
         <v>443</v>
       </c>
       <c r="I116" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J116" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K116"/>
       <c r="L116"/>
@@ -11060,10 +11060,10 @@
         <v>439</v>
       </c>
       <c r="I117" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J117" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K117"/>
       <c r="L117"/>
@@ -11110,10 +11110,10 @@
         <v>443</v>
       </c>
       <c r="I118" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J118" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K118"/>
       <c r="L118"/>
@@ -11260,7 +11260,7 @@
         <v>439</v>
       </c>
       <c r="I121" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J121" t="s">
         <v>452</v>
@@ -11310,10 +11310,10 @@
         <v>443</v>
       </c>
       <c r="I122" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J122" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K122"/>
       <c r="L122"/>
@@ -11360,10 +11360,10 @@
         <v>443</v>
       </c>
       <c r="I123" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J123" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K123"/>
       <c r="L123"/>
@@ -11410,10 +11410,10 @@
         <v>443</v>
       </c>
       <c r="I124" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J124" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K124"/>
       <c r="L124"/>
@@ -11460,10 +11460,10 @@
         <v>443</v>
       </c>
       <c r="I125" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J125" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K125"/>
       <c r="L125"/>
@@ -11510,7 +11510,7 @@
         <v>460</v>
       </c>
       <c r="I126" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J126" t="s">
         <v>461</v>
@@ -11610,7 +11610,7 @@
         <v>257</v>
       </c>
       <c r="I128" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J128" t="s">
         <v>471</v>
@@ -11710,7 +11710,7 @@
         <v>477</v>
       </c>
       <c r="I130" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J130" t="s">
         <v>478</v>
@@ -11860,7 +11860,7 @@
         <v>482</v>
       </c>
       <c r="I133" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J133" t="s">
         <v>489</v>
@@ -12710,7 +12710,7 @@
         <v>531</v>
       </c>
       <c r="I150" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J150" t="s">
         <v>538</v>
@@ -13206,10 +13206,10 @@
         <v>19</v>
       </c>
       <c r="I160" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J160" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K160"/>
       <c r="L160"/>
@@ -13218,10 +13218,10 @@
         <v>19</v>
       </c>
       <c r="O160" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="P160" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="Q160" s="2" t="n">
         <v>36113</v>
@@ -13256,7 +13256,7 @@
         <v>67</v>
       </c>
       <c r="I161" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J161" t="s">
         <v>567</v>
@@ -13556,7 +13556,7 @@
         <v>577</v>
       </c>
       <c r="I167" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="J167" t="s">
         <v>589</v>
@@ -13970,16 +13970,16 @@
         <v>19</v>
       </c>
       <c r="O175" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P175" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q175" s="2" t="n">
         <v>43888</v>
       </c>
       <c r="R175" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="176">
@@ -14008,7 +14008,7 @@
         <v>609</v>
       </c>
       <c r="I176" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J176" t="s">
         <v>19</v>
@@ -14025,13 +14025,13 @@
         <v>574</v>
       </c>
       <c r="P176" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q176" s="2" t="n">
         <v>43888</v>
       </c>
       <c r="R176" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="177">
@@ -14077,13 +14077,13 @@
         <v>574</v>
       </c>
       <c r="P177" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q177" s="2" t="n">
         <v>43889</v>
       </c>
       <c r="R177" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="178">
@@ -14129,13 +14129,13 @@
         <v>574</v>
       </c>
       <c r="P178" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q178" s="2" t="n">
         <v>43889</v>
       </c>
       <c r="R178" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="179">
@@ -14178,16 +14178,16 @@
         <v>19</v>
       </c>
       <c r="O179" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P179" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q179" s="2" t="n">
         <v>43886</v>
       </c>
       <c r="R179" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="180">
@@ -14230,16 +14230,16 @@
         <v>19</v>
       </c>
       <c r="O180" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P180" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q180" s="2" t="n">
         <v>43889</v>
       </c>
       <c r="R180" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="181">
@@ -14282,16 +14282,16 @@
         <v>19</v>
       </c>
       <c r="O181" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P181" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q181" s="2" t="n">
         <v>43889</v>
       </c>
       <c r="R181" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="182">
@@ -14334,16 +14334,16 @@
         <v>19</v>
       </c>
       <c r="O182" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="P182" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q182" s="2" t="n">
         <v>43889</v>
       </c>
       <c r="R182" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="183">
@@ -14372,7 +14372,7 @@
         <v>629</v>
       </c>
       <c r="I183" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J183" t="s">
         <v>630</v>
@@ -14422,10 +14422,10 @@
         <v>633</v>
       </c>
       <c r="I184" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J184" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K184"/>
       <c r="L184"/>
@@ -14526,7 +14526,7 @@
         <v>644</v>
       </c>
       <c r="I186" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J186" t="s">
         <v>645</v>
@@ -14626,7 +14626,7 @@
         <v>644</v>
       </c>
       <c r="I188" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J188" t="s">
         <v>651</v>
@@ -14676,7 +14676,7 @@
         <v>644</v>
       </c>
       <c r="I189" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J189" t="s">
         <v>656</v>
@@ -14888,10 +14888,10 @@
         <v>19</v>
       </c>
       <c r="O193" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="P193" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="Q193" s="2" t="n">
         <v>41927</v>
@@ -14941,7 +14941,7 @@
         <v>676</v>
       </c>
       <c r="P194" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="Q194" s="2" t="n">
         <v>42217</v>
@@ -14988,10 +14988,10 @@
         <v>19</v>
       </c>
       <c r="O195" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="P195" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="Q195" s="2" t="n">
         <v>42315</v>
@@ -15034,10 +15034,10 @@
         <v>19</v>
       </c>
       <c r="O196" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="P196" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
       <c r="Q196" s="2" t="n">
         <v>42644</v>
@@ -18129,7 +18129,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B17" t="n">
         <v>13.1746849175394</v>
@@ -18206,7 +18206,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B18" t="n">
         <v>9.55773190168653</v>
@@ -18285,7 +18285,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B19" t="n">
         <v>41.3400323241401</v>
@@ -18368,7 +18368,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B20" t="n">
         <v>-53.4109250488223</v>
@@ -18451,7 +18451,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B21" t="n">
         <v>-10.2771111668864</v>
@@ -18534,7 +18534,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B22" t="n">
         <v>25.9357530802163</v>
@@ -18617,7 +18617,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B23" t="n">
         <v>-3.16462660761113</v>
@@ -18700,7 +18700,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B24" t="n">
         <v>40.3745304484755</v>
@@ -18783,7 +18783,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B25" t="n">
         <v>-21.0932884956441</v>
@@ -18860,7 +18860,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B26" t="n">
         <v>-144.984886996825</v>
@@ -18943,7 +18943,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B27" t="n">
         <v>16.6812755615846</v>
@@ -19026,7 +19026,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B28" t="n">
         <v>24.8263098568975</v>
@@ -19109,7 +19109,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B29" t="n">
         <v>77.2013679368027</v>
@@ -19188,7 +19188,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B30" t="n">
         <v>-41.5955385346201</v>
@@ -19271,7 +19271,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B31" t="n">
         <v>-23.436194624181</v>
@@ -19354,7 +19354,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B32" t="n">
         <v>-44.2973753116747</v>
@@ -19435,7 +19435,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B33" t="n">
         <v>-46.7564992853078</v>
@@ -19516,7 +19516,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B34" t="n">
         <v>-21.5215091299441</v>
@@ -19597,7 +19597,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B35" t="n">
         <v>2.10907270755336</v>
@@ -19674,7 +19674,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B36" t="n">
         <v>-0.686503973411224</v>
@@ -19757,7 +19757,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B37" t="n">
         <v>-24.1845504719225</v>
@@ -19840,7 +19840,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B38" t="n">
         <v>13.8500035499035</v>
@@ -19923,7 +19923,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B39" t="n">
         <v>-54.3947793744293</v>
@@ -20006,7 +20006,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B40" t="n">
         <v>-8.59085411020072</v>
@@ -20081,7 +20081,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B41" t="n">
         <v>-21.3979293131267</v>
@@ -20156,7 +20156,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B42" t="n">
         <v>-11.9535715423763</v>
@@ -20233,7 +20233,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B43" t="n">
         <v>-0.71244249998194</v>
@@ -20316,7 +20316,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B44" t="n">
         <v>1.47385974619864</v>
@@ -20399,7 +20399,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B45" t="n">
         <v>15.6208088699728</v>
@@ -20474,7 +20474,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="B46" t="n">
         <v>-35.7445651670853</v>
@@ -20557,7 +20557,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>187</v>
+        <v>82</v>
       </c>
       <c r="B47" t="n">
         <v>1.073493257406</v>
@@ -32915,7 +32915,7 @@
         <v>30.9542099501434</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E17" t="s">
         <v>797</v>

</xml_diff>